<commit_message>
fix misaligned michigan orgs
</commit_message>
<xml_diff>
--- a/data/copy.xlsx
+++ b/data/copy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="125">
   <si>
     <t>key</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>PAC</t>
+  </si>
+  <si>
+    <t>African-American</t>
   </si>
   <si>
     <t>Climate</t>
@@ -813,12 +816,12 @@
         <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>39</v>
@@ -829,20 +832,20 @@
         <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>44</v>
@@ -853,12 +856,12 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>47</v>
@@ -1053,44 +1056,44 @@
         <v>71</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>81</v>
@@ -1117,12 +1120,12 @@
         <v>84</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>86</v>
@@ -1158,6 +1161,14 @@
       </c>
       <c r="B50" s="1" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1182,71 +1193,71 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" s="6">
         <v>1.38837436154588E14</v>
@@ -1254,78 +1265,78 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B12" s="8"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B13" s="8"/>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B14" s="8"/>
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B15" s="8"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B16" s="8"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B17" s="8"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22">
@@ -1351,34 +1362,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>